<commit_message>
add ending zeros, draw line
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <r>
       <rPr>
@@ -217,6 +217,21 @@
   </si>
   <si>
     <t xml:space="preserve">Cons: 0.3, stroke:0.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32sktech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cons: 0.021, kl: 0.018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include the ending (0,0)</t>
   </si>
 </sst>
 </file>
@@ -435,22 +450,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5663265306122"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="6.61224489795918"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="35.234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.8265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,6 +719,37 @@
         <v>38</v>
       </c>
     </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="7" t="n">
+        <v>43318</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>30000</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="M22" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="7" t="n">
+        <v>43319</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
fix bug train high rnn
</commit_message>
<xml_diff>
--- a/exp_notes.xlsx
+++ b/exp_notes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <r>
       <rPr>
@@ -56,7 +56,7 @@
     <t xml:space="preserve">目的</t>
   </si>
   <si>
-    <t xml:space="preserve">模型名称</t>
+    <t xml:space="preserve">Lambda</t>
   </si>
   <si>
     <t xml:space="preserve">Clip</t>
@@ -264,19 +264,58 @@
     <t xml:space="preserve">2-6</t>
   </si>
   <si>
+    <t xml:space="preserve">loc=2, kl=0.5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cons:0.022, kl:0.053</t>
   </si>
   <si>
-    <t xml:space="preserve">Lambda_loc=2, Lambda_kl=0.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">2-7</t>
   </si>
   <si>
+    <t xml:space="preserve">loc=1, kl=0.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cons:0.016 , kl:0.06 </t>
   </si>
   <si>
-    <t xml:space="preserve">Lambda_loc=1, Lambda_kl=0.3</t>
+    <t xml:space="preserve">3-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug when concate sketchInput</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loc=0.1,kl=0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eof=0.1, kl=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kl=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recons_High, KL_High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[40000, 55000]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kl=0.01</t>
   </si>
 </sst>
 </file>
@@ -495,20 +534,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M36" activeCellId="0" sqref="M36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0612244897959"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3928571428571"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.3010204081633"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="6.0765306122449"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.44387755102041"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="34.4234693877551"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="8.50510204081633"/>
   </cols>
@@ -773,6 +814,9 @@
       <c r="B22" s="7" t="n">
         <v>43318</v>
       </c>
+      <c r="F22" s="0" t="n">
+        <v>0.1</v>
+      </c>
       <c r="I22" s="0" t="s">
         <v>40</v>
       </c>
@@ -849,13 +893,16 @@
       <c r="A27" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="B27" s="7" t="n">
+        <v>43321</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="K27" s="0" t="n">
         <v>256</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="N27" s="0" t="s">
         <v>55</v>
       </c>
     </row>
@@ -863,11 +910,72 @@
       <c r="A28" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="B28" s="7" t="n">
+        <v>43321</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>57</v>
+      </c>
       <c r="M28" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="N28" s="0" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="7" t="n">
+        <v>43322</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>60000</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>